<commit_message>
fixed alcoholic beverages lookup
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/food commodity to food group table V2.xlsx
+++ b/data-raw/NutrientData/food commodity to food group table V2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/nutrientModeling/data-raw/NutrientData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/nutmod/data-raw/NutrientData/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,6 +16,9 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="154">
   <si>
     <t>Description</t>
   </si>
@@ -480,6 +483,12 @@
   </si>
   <si>
     <t>staple code</t>
+  </si>
+  <si>
+    <t>alcohol</t>
+  </si>
+  <si>
+    <t>alcoholic beverage</t>
   </si>
 </sst>
 </file>
@@ -1059,18 +1068,18 @@
         <v>100</v>
       </c>
       <c r="D2" s="6" t="str">
-        <f>VLOOKUP(C2,F$2:G$14,2)</f>
+        <f>VLOOKUP(C2,F$2:G$15,2)</f>
         <v>fruits</v>
       </c>
       <c r="E2" s="6" t="str">
-        <f>VLOOKUP(D2,G$2:H$14,2)</f>
-        <v>nonstaple</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>110</v>
+        <f>VLOOKUP(D2,G$2:H$15,2)</f>
+        <v>nonstaple</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>119</v>
@@ -1087,21 +1096,21 @@
         <v>95</v>
       </c>
       <c r="D3" s="6" t="str">
-        <f>VLOOKUP(C3,F$2:G$14,2)</f>
+        <f t="shared" ref="D3:D62" si="0">VLOOKUP(C3,F$2:G$15,2)</f>
         <v>cereals</v>
       </c>
       <c r="E3" s="6" t="str">
-        <f t="shared" ref="E3:E62" si="0">VLOOKUP(D3,G$2:H$14,2)</f>
+        <f t="shared" ref="E3:E62" si="1">VLOOKUP(D3,G$2:H$15,2)</f>
         <v>staple</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1115,21 +1124,21 @@
         <v>96</v>
       </c>
       <c r="D4" s="6" t="str">
-        <f>VLOOKUP(C4,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>pulses</v>
       </c>
       <c r="E4" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>staple</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1143,18 +1152,18 @@
         <v>102</v>
       </c>
       <c r="D5" s="6" t="str">
-        <f>VLOOKUP(C5,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>meats</v>
       </c>
       <c r="E5" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="H5" s="11" t="s">
         <v>119</v>
@@ -1171,18 +1180,18 @@
         <v>103</v>
       </c>
       <c r="D6" s="6" t="str">
-        <f>VLOOKUP(C6,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>beverages</v>
       </c>
       <c r="E6" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="H6" s="11" t="s">
         <v>119</v>
@@ -1199,18 +1208,18 @@
         <v>98</v>
       </c>
       <c r="D7" s="6" t="str">
-        <f>VLOOKUP(C7,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>roots</v>
       </c>
       <c r="E7" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>staple</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="H7" s="11" t="s">
         <v>119</v>
@@ -1227,18 +1236,18 @@
         <v>96</v>
       </c>
       <c r="D8" s="6" t="str">
-        <f>VLOOKUP(C8,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>pulses</v>
       </c>
       <c r="E8" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>staple</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>119</v>
@@ -1255,18 +1264,18 @@
         <v>103</v>
       </c>
       <c r="D9" s="6" t="str">
-        <f>VLOOKUP(C9,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>beverages</v>
       </c>
       <c r="E9" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>119</v>
@@ -1283,18 +1292,18 @@
         <v>96</v>
       </c>
       <c r="D10" s="6" t="str">
-        <f>VLOOKUP(C10,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>pulses</v>
       </c>
       <c r="E10" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>staple</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>119</v>
@@ -1311,21 +1320,21 @@
         <v>97</v>
       </c>
       <c r="D11" s="6" t="str">
-        <f>VLOOKUP(C11,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>eggs</v>
       </c>
       <c r="E11" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1339,18 +1348,18 @@
         <v>104</v>
       </c>
       <c r="D12" s="6" t="str">
-        <f>VLOOKUP(C12,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>oils</v>
       </c>
       <c r="E12" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>120</v>
@@ -1367,21 +1376,21 @@
         <v>94</v>
       </c>
       <c r="D13" s="6" t="str">
-        <f>VLOOKUP(C13,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>oilSeeds</v>
       </c>
       <c r="E13" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1395,18 +1404,18 @@
         <v>102</v>
       </c>
       <c r="D14" s="6" t="str">
-        <f>VLOOKUP(C14,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>meats</v>
       </c>
       <c r="E14" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="H14" s="11" t="s">
         <v>119</v>
@@ -1423,12 +1432,21 @@
         <v>96</v>
       </c>
       <c r="D15" s="6" t="str">
-        <f>VLOOKUP(C15,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>pulses</v>
       </c>
       <c r="E15" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>staple</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1442,11 +1460,11 @@
         <v>95</v>
       </c>
       <c r="D16" s="6" t="str">
-        <f>VLOOKUP(C16,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>cereals</v>
       </c>
       <c r="E16" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>staple</v>
       </c>
     </row>
@@ -1461,11 +1479,11 @@
         <v>93</v>
       </c>
       <c r="D17" s="6" t="str">
-        <f>VLOOKUP(C17,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>diary</v>
       </c>
       <c r="E17" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -1480,11 +1498,11 @@
         <v>95</v>
       </c>
       <c r="D18" s="6" t="str">
-        <f>VLOOKUP(C18,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>cereals</v>
       </c>
       <c r="E18" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>staple</v>
       </c>
     </row>
@@ -1499,11 +1517,11 @@
         <v>95</v>
       </c>
       <c r="D19" s="6" t="str">
-        <f>VLOOKUP(C19,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>cereals</v>
       </c>
       <c r="E19" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>staple</v>
       </c>
     </row>
@@ -1518,11 +1536,11 @@
         <v>96</v>
       </c>
       <c r="D20" s="6" t="str">
-        <f>VLOOKUP(C20,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>pulses</v>
       </c>
       <c r="E20" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>staple</v>
       </c>
     </row>
@@ -1537,11 +1555,11 @@
         <v>98</v>
       </c>
       <c r="D21" s="6" t="str">
-        <f>VLOOKUP(C21,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>roots</v>
       </c>
       <c r="E21" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>staple</v>
       </c>
     </row>
@@ -1556,11 +1574,11 @@
         <v>95</v>
       </c>
       <c r="D22" s="6" t="str">
-        <f>VLOOKUP(C22,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>cereals</v>
       </c>
       <c r="E22" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>staple</v>
       </c>
     </row>
@@ -1575,11 +1593,11 @@
         <v>96</v>
       </c>
       <c r="D23" s="6" t="str">
-        <f>VLOOKUP(C23,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>pulses</v>
       </c>
       <c r="E23" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>staple</v>
       </c>
     </row>
@@ -1594,11 +1612,11 @@
         <v>104</v>
       </c>
       <c r="D24" s="6" t="str">
-        <f>VLOOKUP(C24,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>oils</v>
       </c>
       <c r="E24" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -1613,11 +1631,11 @@
         <v>98</v>
       </c>
       <c r="D25" s="6" t="str">
-        <f>VLOOKUP(C25,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>roots</v>
       </c>
       <c r="E25" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>staple</v>
       </c>
     </row>
@@ -1632,11 +1650,11 @@
         <v>104</v>
       </c>
       <c r="D26" s="6" t="str">
-        <f>VLOOKUP(C26,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>oils</v>
       </c>
       <c r="E26" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -1651,11 +1669,11 @@
         <v>102</v>
       </c>
       <c r="D27" s="6" t="str">
-        <f>VLOOKUP(C27,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>meats</v>
       </c>
       <c r="E27" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -1670,11 +1688,11 @@
         <v>98</v>
       </c>
       <c r="D28" s="6" t="str">
-        <f>VLOOKUP(C28,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>roots</v>
       </c>
       <c r="E28" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>staple</v>
       </c>
     </row>
@@ -1689,11 +1707,11 @@
         <v>102</v>
       </c>
       <c r="D29" s="6" t="str">
-        <f>VLOOKUP(C29,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>meats</v>
       </c>
       <c r="E29" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -1708,11 +1726,11 @@
         <v>95</v>
       </c>
       <c r="D30" s="6" t="str">
-        <f>VLOOKUP(C30,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>cereals</v>
       </c>
       <c r="E30" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>staple</v>
       </c>
     </row>
@@ -1727,11 +1745,11 @@
         <v>104</v>
       </c>
       <c r="D31" s="6" t="str">
-        <f>VLOOKUP(C31,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>oils</v>
       </c>
       <c r="E31" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -1746,11 +1764,11 @@
         <v>94</v>
       </c>
       <c r="D32" s="6" t="str">
-        <f>VLOOKUP(C32,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>oilSeeds</v>
       </c>
       <c r="E32" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -1765,11 +1783,11 @@
         <v>104</v>
       </c>
       <c r="D33" s="6" t="str">
-        <f>VLOOKUP(C33,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>oils</v>
       </c>
       <c r="E33" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -1784,11 +1802,11 @@
         <v>104</v>
       </c>
       <c r="D34" s="6" t="str">
-        <f>VLOOKUP(C34,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>oils</v>
       </c>
       <c r="E34" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -1803,11 +1821,11 @@
         <v>94</v>
       </c>
       <c r="D35" s="6" t="str">
-        <f>VLOOKUP(C35,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>oilSeeds</v>
       </c>
       <c r="E35" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -1822,11 +1840,11 @@
         <v>95</v>
       </c>
       <c r="D36" s="6" t="str">
-        <f>VLOOKUP(C36,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>cereals</v>
       </c>
       <c r="E36" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>staple</v>
       </c>
     </row>
@@ -1841,11 +1859,11 @@
         <v>94</v>
       </c>
       <c r="D37" s="6" t="str">
-        <f>VLOOKUP(C37,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>oilSeeds</v>
       </c>
       <c r="E37" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -1860,11 +1878,11 @@
         <v>100</v>
       </c>
       <c r="D38" s="6" t="str">
-        <f>VLOOKUP(C38,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>fruits</v>
       </c>
       <c r="E38" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -1879,11 +1897,11 @@
         <v>105</v>
       </c>
       <c r="D39" s="6" t="str">
-        <f>VLOOKUP(C39,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>sweeteners</v>
       </c>
       <c r="E39" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -1898,11 +1916,11 @@
         <v>98</v>
       </c>
       <c r="D40" s="6" t="str">
-        <f>VLOOKUP(C40,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>roots</v>
       </c>
       <c r="E40" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>staple</v>
       </c>
     </row>
@@ -1917,11 +1935,11 @@
         <v>103</v>
       </c>
       <c r="D41" s="6" t="str">
-        <f>VLOOKUP(C41,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>beverages</v>
       </c>
       <c r="E41" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -1936,11 +1954,11 @@
         <v>100</v>
       </c>
       <c r="D42" s="6" t="str">
-        <f>VLOOKUP(C42,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>fruits</v>
       </c>
       <c r="E42" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -1955,11 +1973,11 @@
         <v>94</v>
       </c>
       <c r="D43" s="6" t="str">
-        <f>VLOOKUP(C43,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>oilSeeds</v>
       </c>
       <c r="E43" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -1974,11 +1992,11 @@
         <v>104</v>
       </c>
       <c r="D44" s="6" t="str">
-        <f>VLOOKUP(C44,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>oils</v>
       </c>
       <c r="E44" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -1993,11 +2011,11 @@
         <v>101</v>
       </c>
       <c r="D45" s="6" t="str">
-        <f>VLOOKUP(C45,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>vegetables</v>
       </c>
       <c r="E45" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -2012,11 +2030,11 @@
         <v>95</v>
       </c>
       <c r="D46" s="6" t="str">
-        <f>VLOOKUP(C46,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>cereals</v>
       </c>
       <c r="E46" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>staple</v>
       </c>
     </row>
@@ -2031,11 +2049,11 @@
         <v>98</v>
       </c>
       <c r="D47" s="6" t="str">
-        <f>VLOOKUP(C47,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>roots</v>
       </c>
       <c r="E47" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>staple</v>
       </c>
     </row>
@@ -2050,11 +2068,11 @@
         <v>99</v>
       </c>
       <c r="D48" s="6" t="str">
-        <f>VLOOKUP(C48,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>fish</v>
       </c>
       <c r="E48" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -2069,11 +2087,11 @@
         <v>99</v>
       </c>
       <c r="D49" s="6" t="str">
-        <f t="shared" ref="D49:D62" si="1">VLOOKUP(C49,F$2:G$14,2)</f>
+        <f t="shared" si="0"/>
         <v>fish</v>
       </c>
       <c r="E49" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -2088,11 +2106,11 @@
         <v>99</v>
       </c>
       <c r="D50" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>fish</v>
       </c>
       <c r="E50" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -2107,11 +2125,11 @@
         <v>99</v>
       </c>
       <c r="D51" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>fish</v>
       </c>
       <c r="E51" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -2126,11 +2144,11 @@
         <v>99</v>
       </c>
       <c r="D52" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>fish</v>
       </c>
       <c r="E52" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -2145,11 +2163,11 @@
         <v>99</v>
       </c>
       <c r="D53" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>fish</v>
       </c>
       <c r="E53" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -2164,11 +2182,11 @@
         <v>99</v>
       </c>
       <c r="D54" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>fish</v>
       </c>
       <c r="E54" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -2183,11 +2201,11 @@
         <v>99</v>
       </c>
       <c r="D55" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>fish</v>
       </c>
       <c r="E55" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -2202,11 +2220,11 @@
         <v>99</v>
       </c>
       <c r="D56" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>fish</v>
       </c>
       <c r="E56" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -2221,11 +2239,11 @@
         <v>104</v>
       </c>
       <c r="D57" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>oils</v>
       </c>
       <c r="E57" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -2237,14 +2255,14 @@
         <v>146</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>103</v>
+        <v>153</v>
       </c>
       <c r="D58" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>beverages</v>
+        <f t="shared" si="0"/>
+        <v>alcohol</v>
       </c>
       <c r="E58" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -2256,14 +2274,14 @@
         <v>147</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>103</v>
+        <v>153</v>
       </c>
       <c r="D59" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>beverages</v>
+        <f t="shared" si="0"/>
+        <v>alcohol</v>
       </c>
       <c r="E59" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -2278,11 +2296,11 @@
         <v>103</v>
       </c>
       <c r="D60" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>beverages</v>
       </c>
       <c r="E60" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -2297,11 +2315,11 @@
         <v>102</v>
       </c>
       <c r="D61" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>meats</v>
       </c>
       <c r="E61" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
@@ -2316,11 +2334,11 @@
         <v>101</v>
       </c>
       <c r="D62" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>vegetables</v>
       </c>
       <c r="E62" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed spelling of dairy in food group lookup spreadsheet. Figured out that I need to do aggregation in the alcohol and fish management code. Modified nutCalcsProcessing by moving the graphing code to another script.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/food commodity to food group table V2.xlsx
+++ b/data-raw/NutrientData/food commodity to food group table V2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27011"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="153">
   <si>
     <t>Description</t>
   </si>
@@ -360,9 +360,6 @@
   </si>
   <si>
     <t>beverages</t>
-  </si>
-  <si>
-    <t>diary</t>
   </si>
   <si>
     <t>oils</t>
@@ -1015,7 +1012,7 @@
   <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E62"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1033,7 +1030,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1045,7 +1042,7 @@
         <v>108</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>106</v>
@@ -1054,7 +1051,7 @@
         <v>109</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1076,13 +1073,13 @@
         <v>nonstaple</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1110,7 +1107,7 @@
         <v>110</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1138,7 +1135,7 @@
         <v>95</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1163,10 +1160,10 @@
         <v>93</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1194,7 +1191,7 @@
         <v>97</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1219,10 +1216,10 @@
         <v>104</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1250,7 +1247,7 @@
         <v>99</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1278,7 +1275,7 @@
         <v>100</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1303,10 +1300,10 @@
         <v>102</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1331,10 +1328,10 @@
         <v>94</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1362,7 +1359,7 @@
         <v>96</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1387,10 +1384,10 @@
         <v>98</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1415,10 +1412,10 @@
         <v>105</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1446,7 +1443,7 @@
         <v>101</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1478,9 +1475,8 @@
       <c r="C17" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D17" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>diary</v>
+      <c r="D17" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="E17" s="6" t="str">
         <f t="shared" si="1"/>
@@ -2059,10 +2055,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>99</v>
@@ -2078,10 +2074,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>99</v>
@@ -2097,10 +2093,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>99</v>
@@ -2116,10 +2112,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>99</v>
@@ -2135,10 +2131,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>99</v>
@@ -2154,10 +2150,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>99</v>
@@ -2173,10 +2169,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>99</v>
@@ -2192,10 +2188,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>99</v>
@@ -2211,10 +2207,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>99</v>
@@ -2230,10 +2226,10 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>104</v>
@@ -2249,13 +2245,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2268,13 +2264,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D59" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2287,10 +2283,10 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>103</v>
@@ -2306,10 +2302,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>102</v>
@@ -2325,10 +2321,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>101</v>

</xml_diff>